<commit_message>
Object Recognition module update
</commit_message>
<xml_diff>
--- a/Accuracy-data.xlsx
+++ b/Accuracy-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://habibuniversity-my.sharepoint.com/personal/ah04318_st_habib_edu_pk/Documents/Habib University/Final Year Project - Parwaaz/Object_Recognition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0A9AE66-34C0-4FA0-85C1-F8D69968AB58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB072A-E06B-4F94-B64B-98CE36D2726D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{71818E5E-8792-4ABD-94DD-29B9E79B15E2}"/>
+    <workbookView xWindow="7065" yWindow="3270" windowWidth="24795" windowHeight="13725" xr2:uid="{71818E5E-8792-4ABD-94DD-29B9E79B15E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,101 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+  <si>
+    <t>Day Light Testing</t>
+  </si>
+  <si>
+    <t>Video name</t>
+  </si>
+  <si>
+    <t>Accuracy average</t>
+  </si>
+  <si>
+    <t>Night/dark Time Testing</t>
+  </si>
+  <si>
+    <t>carlight1</t>
+  </si>
+  <si>
+    <t>carlight2</t>
+  </si>
+  <si>
+    <t>cardim1</t>
+  </si>
+  <si>
+    <t>cardim2</t>
+  </si>
+  <si>
+    <t>cardim3</t>
+  </si>
+  <si>
+    <t>airplanelight1</t>
+  </si>
+  <si>
+    <t>airplanelight2</t>
+  </si>
+  <si>
+    <t>airplanelight3</t>
+  </si>
+  <si>
+    <t>airplanedim1</t>
+  </si>
+  <si>
+    <t>airplanedim2</t>
+  </si>
+  <si>
+    <t>motorcyclelight1</t>
+  </si>
+  <si>
+    <t>motorcycledim1</t>
+  </si>
+  <si>
+    <t>buslight1</t>
+  </si>
+  <si>
+    <t>busdim1</t>
+  </si>
+  <si>
+    <t>buslight2</t>
+  </si>
+  <si>
+    <t>bicyclelight1</t>
+  </si>
+  <si>
+    <t>bicycledim1</t>
+  </si>
+  <si>
+    <t>trainlight1</t>
+  </si>
+  <si>
+    <t>traindim1</t>
+  </si>
+  <si>
+    <t>boat light1</t>
+  </si>
+  <si>
+    <t>boatdim1</t>
+  </si>
+  <si>
+    <t>trucklight1</t>
+  </si>
+  <si>
+    <t>truckdim1</t>
+  </si>
+  <si>
+    <t>truckdim2</t>
+  </si>
+  <si>
+    <t>treelight1</t>
+  </si>
+  <si>
+    <t>treedim1</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,8 +150,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,17 +470,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9C7F72-0615-4146-8B10-AF74C11E81FE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.90190000000000003</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>0.83840000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.78080000000000005</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>0.87329999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>0.94040000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.94279999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.96289999999999998</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>0.93289999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.98119999999999996</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>0.97289999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <v>0.76329999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>0.94130000000000003</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12">
+        <v>0.88966999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0.96750000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>0.66169999999999995</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <v>0.90700000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>0.61470000000000002</v>
+      </c>
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17">
+        <v>0.86519999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>0.93979999999999997</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19">
+        <v>0.68679999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>0.89929999999999999</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21">
+        <v>0.77959999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22">
+        <v>0.79669999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>0.56969999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24">
+        <v>0.68530000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E5E39FFE2E405C4E87539D4CEEF93F3D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="658e3634d9ac29fc2e9b323d7f0f1da6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4c54cfa4-7532-4044-9fb3-32446fd9eb09" xmlns:ns4="7e0a9eca-1dd2-44e1-a6ce-62f6c8de3083" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2358d3dcdc7367576536c18ab3fbee5" ns3:_="" ns4:_="">
     <xsd:import namespace="4c54cfa4-7532-4044-9fb3-32446fd9eb09"/>
@@ -604,7 +937,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -613,13 +946,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A330BB35-88F7-4E29-B3F3-885DBCA3479D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4c54cfa4-7532-4044-9fb3-32446fd9eb09"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7e0a9eca-1dd2-44e1-a6ce-62f6c8de3083"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{687B7591-B09F-4522-B9DC-C8B22ADAB283}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -638,27 +982,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9290419D-B989-4AFC-AC9B-EEAAE3A30A07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A330BB35-88F7-4E29-B3F3-885DBCA3479D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4c54cfa4-7532-4044-9fb3-32446fd9eb09"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7e0a9eca-1dd2-44e1-a6ce-62f6c8de3083"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>